<commit_message>
~ minor changes, methods, ccfgs
</commit_message>
<xml_diff>
--- a/examples/oucru/oucru-06dx/resources/outputs/templates/ccfgs_06dx_data_fixed.xlsx
+++ b/examples/oucru/oucru-06dx/resources/outputs/templates/ccfgs_06dx_data_fixed.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kelda\Desktop\repositories\github\datablend\main\examples\oucru\oucru-06dx\resources\outputs\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B348A1F-BE68-4B2E-91A3-32418888CFA1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41EB4B6D-CA91-4A66-9AD6-EE50B4E94196}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25530" yWindow="1260" windowWidth="20325" windowHeight="16470" firstSheet="1" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25650" yWindow="825" windowWidth="23730" windowHeight="16470" firstSheet="5" activeTab="17" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SCR" sheetId="1" r:id="rId1"/>
@@ -2268,9 +2268,6 @@
     <t>{1: 1, 2: 2, 3: 3}</t>
   </si>
   <si>
-    <t>{2: 3, 1: 1, 3: 3}</t>
-  </si>
-  <si>
     <t>indirect_elisa_result</t>
   </si>
   <si>
@@ -2278,6 +2275,9 @@
   </si>
   <si>
     <t>{1: 'Placebo - Low Dose', 2: 'Placebo - High Dose', 3: 'Steroids - Low Dose', 4: 'Steroids - High Dose'}</t>
+  </si>
+  <si>
+    <t>{2: False, 1: True, 3: None}</t>
   </si>
 </sst>
 </file>
@@ -3754,7 +3754,7 @@
   <dimension ref="A1:J24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5581,7 +5581,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I38" sqref="I38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5798,8 +5798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10:E13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6032,7 +6032,7 @@
         <v>599</v>
       </c>
       <c r="B12" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="C12" t="s">
         <v>66</v>
@@ -6058,7 +6058,7 @@
         <v>66</v>
       </c>
       <c r="D13" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="E13" t="s">
         <v>560</v>
@@ -6107,8 +6107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6210,7 +6210,7 @@
         <v>616</v>
       </c>
       <c r="B5" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="C5" t="s">
         <v>101</v>
@@ -6233,7 +6233,7 @@
         <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="E6" t="s">
         <v>618</v>
@@ -8500,8 +8500,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K43"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>